<commit_message>
Included JavaScript topics - String Literal and DOM
</commit_message>
<xml_diff>
--- a/media-data.xlsx
+++ b/media-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my-academy\learning-videos\fsd-part2-ng-java\fsd-part2-ng-java-draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0768C23-CFAB-405D-9D66-11C7DC863E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8438A4B-01BF-45FE-B465-5470F4D424EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B52A62E0-993B-4205-95A1-E40361DFFE6B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{B52A62E0-993B-4205-95A1-E40361DFFE6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="260">
   <si>
     <t>id</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Create menu.html</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=q8ky03I1Nco</t>
-  </si>
-  <si>
     <t>Remove row div from menu.html</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Bootstrap - Learn Collapse Component</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=Fu0_60zflCY</t>
-  </si>
-  <si>
     <t>View Navigation Links in Mobile</t>
   </si>
   <si>
@@ -491,214 +485,334 @@
     <t>0726</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=oPGR86X_vUU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=xdzwgV3e4vc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=AbXw9Z4VlzM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=WpfMA88QsvA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=-6OSCkwBBHs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=ibTB2ebbN5c</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=pCzddolnEKs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=MmWBagEKbFI</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=v6cT9k7vY3w</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=BGHa1grXJpg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=yXwK-1pOIqQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=WJnrl4T0h9c</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=J_4SwOUwvQ8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=M2dddUGHlY8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=fyBfSvrhtnc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=c4rTPVgMrPA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=Oab8xlbKOEw</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=ysY09zoLfog</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=nckQUcQsXZc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=3ljDgKO0LBE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=S0UWt3-eqqM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=j0dWro77DU4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=5dzhgvQ-lRE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=fbh9CoTBoJQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=Orn7NYUs6L0</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=o5ORkF7NtpA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=QiHFhi_BNts</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=ZLy9zh70EyM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=klnVXGhaHjg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=itBj04xeqm8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=0nOQqFQ7WBU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=l3zpJI8G7ps</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=2MiCoBxkEtU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=M8wnGjtjnSI</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=S58OiLjXc3o</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=olWVEbDQ2Wc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=uV8STkwtbjs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=FltntsxQEXA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=CBWMltjkSZs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=_D_UiJ-Tt_o</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=5t0GG2Xsw64</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=UmrCO5dfLuw</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=8-gpAIogBp4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=APiqAgI6bDc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=-nYDHQUtBek</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=3r7CDoCcI7o</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=TyWDMWmFTtY</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=5-Ui8hN5ot4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=xu8xJ6fygM4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=oFN9rpHQPaU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=AH6fUZa2d7w</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=uc8UXTGIxes</t>
-  </si>
-  <si>
     <t>0727</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=jtBtHNy27Ds</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=Wc0RdKDtKas</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=HDfRMTO9p0c</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=KPOq3lP-VFg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=8808fwHl8jE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=C0KlqWbYGwI</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=kHgldOcCdY8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=OGfC1tmf838</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=Jmm5hwEqnAM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=JfqeVBe7c1o</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=YK0f6ZmKEOM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=6VvfvfCj88A</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=DJEPi-yqtxI</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=aM1iSdpTbfA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=2rimEkw0lc8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=ErvFlEYNWmQ</t>
-  </si>
-  <si>
     <t>seq</t>
+  </si>
+  <si>
+    <t>JavaScript - Console Log and String Literal</t>
+  </si>
+  <si>
+    <t>0801</t>
+  </si>
+  <si>
+    <t>0802</t>
+  </si>
+  <si>
+    <t>0803</t>
+  </si>
+  <si>
+    <t>0804</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>0806</t>
+  </si>
+  <si>
+    <t>0807</t>
+  </si>
+  <si>
+    <t>Display menu item names demo example</t>
+  </si>
+  <si>
+    <t>Create 'javascript' folder</t>
+  </si>
+  <si>
+    <t>Create folder for learning "String Literals"</t>
+  </si>
+  <si>
+    <t>Implement menu item display using console</t>
+  </si>
+  <si>
+    <t>Check menu item display in console</t>
+  </si>
+  <si>
+    <t>Console log explained</t>
+  </si>
+  <si>
+    <t>String Literal explained</t>
+  </si>
+  <si>
+    <t>Create file of DOM learning</t>
+  </si>
+  <si>
+    <t>Include div tag for displaying menu item names</t>
+  </si>
+  <si>
+    <t>Include JavaScript statement to modify div content</t>
+  </si>
+  <si>
+    <t>Code Execution Flow and Single Line Comments</t>
+  </si>
+  <si>
+    <t>DOM Explained</t>
+  </si>
+  <si>
+    <t>0901</t>
+  </si>
+  <si>
+    <t>0902</t>
+  </si>
+  <si>
+    <t>0903</t>
+  </si>
+  <si>
+    <t>0904</t>
+  </si>
+  <si>
+    <t>0905</t>
+  </si>
+  <si>
+    <t>JavaScript - Document Object Model (DOM)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=q8ky03I1Nco</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=Fu0_60zflCY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=oPGR86X_vUU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=xdzwgV3e4vc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=AbXw9Z4VlzM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=WpfMA88QsvA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=-6OSCkwBBHs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=ibTB2ebbN5c</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=pCzddolnEKs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=MmWBagEKbFI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=v6cT9k7vY3w</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=BGHa1grXJpg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=yXwK-1pOIqQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=WJnrl4T0h9c</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=J_4SwOUwvQ8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=M2dddUGHlY8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=fyBfSvrhtnc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=c4rTPVgMrPA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=Oab8xlbKOEw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=ysY09zoLfog</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=nckQUcQsXZc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=3ljDgKO0LBE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=S0UWt3-eqqM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=j0dWro77DU4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=5dzhgvQ-lRE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=fbh9CoTBoJQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=Orn7NYUs6L0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=o5ORkF7NtpA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=QiHFhi_BNts</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=ZLy9zh70EyM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=klnVXGhaHjg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=itBj04xeqm8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=0nOQqFQ7WBU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=l3zpJI8G7ps</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=2MiCoBxkEtU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=M8wnGjtjnSI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=S58OiLjXc3o</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=olWVEbDQ2Wc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=uV8STkwtbjs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=FltntsxQEXA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=CBWMltjkSZs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=_D_UiJ-Tt_o</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=5t0GG2Xsw64</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=UmrCO5dfLuw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=8-gpAIogBp4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=APiqAgI6bDc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=-nYDHQUtBek</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=3r7CDoCcI7o</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=TyWDMWmFTtY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=5-Ui8hN5ot4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=xu8xJ6fygM4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=oFN9rpHQPaU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=AH6fUZa2d7w</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=uc8UXTGIxes</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=jtBtHNy27Ds</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=Wc0RdKDtKas</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=HDfRMTO9p0c</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=KPOq3lP-VFg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=8808fwHl8jE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=C0KlqWbYGwI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=kHgldOcCdY8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=OGfC1tmf838</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=Jmm5hwEqnAM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=JfqeVBe7c1o</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=YK0f6ZmKEOM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=6VvfvfCj88A</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=DJEPi-yqtxI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=aM1iSdpTbfA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=2rimEkw0lc8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=ErvFlEYNWmQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=m2mxY2vp1u4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=ktpKlKTiGO4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=IRjMUt-jNio</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=fwffoPQVeYE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=1fRvMJoJGGI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=IOXIZmzSDx8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=zj8r454LfO4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=pNrWP3BcdTg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=rcQk8M6YGzU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=9PBG6TFJRug</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=JOCHuqvn1_g</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v=c3IhnqGHt88</t>
   </si>
 </sst>
 </file>
@@ -1068,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71224FC-8233-4372-B3AC-ED209CD2EB9B}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1090,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>221</v>
+        <v>151</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1107,13 +1221,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1124,13 +1238,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1141,13 +1255,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1158,13 +1272,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1172,16 +1286,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1189,16 +1303,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1206,16 +1320,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1223,16 +1337,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1240,16 +1354,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
       <c r="E10" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1257,16 +1371,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1274,16 +1388,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1291,16 +1405,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1308,16 +1422,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1325,16 +1439,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>163</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1342,16 +1456,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1359,16 +1473,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1376,16 +1490,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1393,16 +1507,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" t="s">
-        <v>27</v>
-      </c>
       <c r="E19" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1410,16 +1524,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1427,16 +1541,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1444,16 +1558,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1461,16 +1575,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1478,16 +1592,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1495,16 +1609,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1512,16 +1626,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E26" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1529,16 +1643,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1546,16 +1660,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E28" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1563,16 +1677,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E29" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1580,16 +1694,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1597,16 +1711,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E31" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1614,16 +1728,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E32" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1631,16 +1745,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1648,16 +1762,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -1665,16 +1779,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E35" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1682,16 +1796,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E36" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1699,16 +1813,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E37" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1716,16 +1830,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E38" t="s">
-        <v>185</v>
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -1733,16 +1847,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E39" t="s">
-        <v>186</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -1750,16 +1864,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E40" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -1767,16 +1881,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E41" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -1784,16 +1898,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E42" t="s">
-        <v>189</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -1801,16 +1915,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D43" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E43" t="s">
-        <v>190</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -1818,16 +1932,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E44" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -1835,16 +1949,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D45" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E45" t="s">
-        <v>192</v>
+        <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -1852,16 +1966,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>193</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -1869,16 +1983,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D47" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E47" t="s">
-        <v>194</v>
+        <v>222</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -1886,16 +2000,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D48" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D48" t="s">
-        <v>58</v>
-      </c>
       <c r="E48" t="s">
-        <v>195</v>
+        <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
@@ -1903,16 +2017,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D49" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E49" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
@@ -1920,16 +2034,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D50" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E50" t="s">
-        <v>197</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
@@ -1937,16 +2051,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D51" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E51" t="s">
-        <v>198</v>
+        <v>226</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
@@ -1954,16 +2068,16 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D52" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E52" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
@@ -1971,16 +2085,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D53" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E53" t="s">
-        <v>200</v>
+        <v>228</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
@@ -1988,16 +2102,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D54" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E54" t="s">
-        <v>201</v>
+        <v>229</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
@@ -2005,16 +2119,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E55" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
@@ -2022,16 +2136,16 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E56" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
@@ -2039,16 +2153,16 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D57" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E57" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
@@ -2056,16 +2170,16 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D58" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E58" t="s">
-        <v>206</v>
+        <v>233</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
@@ -2073,16 +2187,16 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D59" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E59" t="s">
-        <v>207</v>
+        <v>234</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
@@ -2090,16 +2204,16 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D60" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E60" t="s">
-        <v>208</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
@@ -2107,16 +2221,16 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D61" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E61" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
@@ -2124,16 +2238,16 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D62" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E62" t="s">
-        <v>210</v>
+        <v>237</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
@@ -2141,16 +2255,16 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D63" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E63" t="s">
-        <v>211</v>
+        <v>238</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
@@ -2158,16 +2272,16 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D64" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E64" t="s">
-        <v>212</v>
+        <v>239</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
@@ -2175,16 +2289,16 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D65" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E65" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
@@ -2192,16 +2306,16 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D66" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E66" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
@@ -2209,16 +2323,16 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D67" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E67" t="s">
-        <v>215</v>
+        <v>242</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
@@ -2226,16 +2340,16 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D68" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E68" t="s">
-        <v>216</v>
+        <v>243</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
@@ -2243,16 +2357,16 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D69" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E69" t="s">
-        <v>217</v>
+        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
@@ -2260,16 +2374,16 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D70" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E70" t="s">
-        <v>218</v>
+        <v>245</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
@@ -2277,16 +2391,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D71" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E71" t="s">
-        <v>219</v>
+        <v>246</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
@@ -2294,16 +2408,220 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>204</v>
+        <v>150</v>
       </c>
       <c r="D72" t="s">
+        <v>79</v>
+      </c>
+      <c r="E72" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>152</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D73" t="s">
+        <v>160</v>
+      </c>
+      <c r="E73" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>152</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D74" t="s">
+        <v>161</v>
+      </c>
+      <c r="E74" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D75" t="s">
+        <v>162</v>
+      </c>
+      <c r="E75" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>152</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D76" t="s">
+        <v>163</v>
+      </c>
+      <c r="E76" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>152</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D77" t="s">
+        <v>164</v>
+      </c>
+      <c r="E77" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>152</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D78" t="s">
+        <v>165</v>
+      </c>
+      <c r="E78" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>152</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D79" t="s">
+        <v>166</v>
+      </c>
+      <c r="E79" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>177</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D80" t="s">
+        <v>167</v>
+      </c>
+      <c r="E80" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>177</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D81" t="s">
+        <v>168</v>
+      </c>
+      <c r="E81" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82">
         <v>81</v>
       </c>
-      <c r="E72" t="s">
-        <v>220</v>
+      <c r="B82" t="s">
+        <v>177</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D82" t="s">
+        <v>169</v>
+      </c>
+      <c r="E82" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>177</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D83" t="s">
+        <v>170</v>
+      </c>
+      <c r="E83" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>177</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D84" t="s">
+        <v>171</v>
+      </c>
+      <c r="E84" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed embed url error
</commit_message>
<xml_diff>
--- a/media-data.xlsx
+++ b/media-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my-academy\learning-videos\fsd-part2-ng-java\fsd-part2-ng-java-draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8438A4B-01BF-45FE-B465-5470F4D424EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAB7D2C-697C-4AFC-9B96-1C1C97901DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{B52A62E0-993B-4205-95A1-E40361DFFE6B}"/>
   </bookViews>
@@ -569,250 +569,250 @@
     <t>JavaScript - Document Object Model (DOM)</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/v=q8ky03I1Nco</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=Fu0_60zflCY</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=oPGR86X_vUU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=xdzwgV3e4vc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=AbXw9Z4VlzM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=WpfMA88QsvA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=-6OSCkwBBHs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=ibTB2ebbN5c</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=pCzddolnEKs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=MmWBagEKbFI</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=v6cT9k7vY3w</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=BGHa1grXJpg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=yXwK-1pOIqQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=WJnrl4T0h9c</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=J_4SwOUwvQ8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=M2dddUGHlY8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=fyBfSvrhtnc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=c4rTPVgMrPA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=Oab8xlbKOEw</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=ysY09zoLfog</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=nckQUcQsXZc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=3ljDgKO0LBE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=S0UWt3-eqqM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=j0dWro77DU4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=5dzhgvQ-lRE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=fbh9CoTBoJQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=Orn7NYUs6L0</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=o5ORkF7NtpA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=QiHFhi_BNts</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=ZLy9zh70EyM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=klnVXGhaHjg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=itBj04xeqm8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=0nOQqFQ7WBU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=l3zpJI8G7ps</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=2MiCoBxkEtU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=M8wnGjtjnSI</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=S58OiLjXc3o</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=olWVEbDQ2Wc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=uV8STkwtbjs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=FltntsxQEXA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=CBWMltjkSZs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=_D_UiJ-Tt_o</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=5t0GG2Xsw64</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=UmrCO5dfLuw</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=8-gpAIogBp4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=APiqAgI6bDc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=-nYDHQUtBek</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=3r7CDoCcI7o</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=TyWDMWmFTtY</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=5-Ui8hN5ot4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=xu8xJ6fygM4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=oFN9rpHQPaU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=AH6fUZa2d7w</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=uc8UXTGIxes</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=jtBtHNy27Ds</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=Wc0RdKDtKas</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=HDfRMTO9p0c</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=KPOq3lP-VFg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=8808fwHl8jE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=C0KlqWbYGwI</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=kHgldOcCdY8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=OGfC1tmf838</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=Jmm5hwEqnAM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=JfqeVBe7c1o</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=YK0f6ZmKEOM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=6VvfvfCj88A</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=DJEPi-yqtxI</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=aM1iSdpTbfA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=2rimEkw0lc8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=ErvFlEYNWmQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=m2mxY2vp1u4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=ktpKlKTiGO4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=IRjMUt-jNio</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=fwffoPQVeYE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=1fRvMJoJGGI</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=IOXIZmzSDx8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=zj8r454LfO4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=pNrWP3BcdTg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=rcQk8M6YGzU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=9PBG6TFJRug</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=JOCHuqvn1_g</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/embed/v=c3IhnqGHt88</t>
+    <t>https://www.youtube.com/embed/q8ky03I1Nco</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/Fu0_60zflCY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/oPGR86X_vUU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/xdzwgV3e4vc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/AbXw9Z4VlzM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/WpfMA88QsvA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/-6OSCkwBBHs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/ibTB2ebbN5c</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/pCzddolnEKs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/MmWBagEKbFI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/v6cT9k7vY3w</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/BGHa1grXJpg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/yXwK-1pOIqQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/WJnrl4T0h9c</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/J_4SwOUwvQ8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/M2dddUGHlY8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/fyBfSvrhtnc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/c4rTPVgMrPA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/Oab8xlbKOEw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/ysY09zoLfog</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/nckQUcQsXZc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/3ljDgKO0LBE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/S0UWt3-eqqM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/j0dWro77DU4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/5dzhgvQ-lRE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/fbh9CoTBoJQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/Orn7NYUs6L0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/o5ORkF7NtpA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/QiHFhi_BNts</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/ZLy9zh70EyM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/klnVXGhaHjg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/itBj04xeqm8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/0nOQqFQ7WBU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/l3zpJI8G7ps</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/2MiCoBxkEtU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/M8wnGjtjnSI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/S58OiLjXc3o</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/olWVEbDQ2Wc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/uV8STkwtbjs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/FltntsxQEXA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/CBWMltjkSZs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/_D_UiJ-Tt_o</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/5t0GG2Xsw64</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/UmrCO5dfLuw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/8-gpAIogBp4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/APiqAgI6bDc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/-nYDHQUtBek</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/3r7CDoCcI7o</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/TyWDMWmFTtY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/5-Ui8hN5ot4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/xu8xJ6fygM4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/oFN9rpHQPaU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/AH6fUZa2d7w</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/uc8UXTGIxes</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/jtBtHNy27Ds</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/Wc0RdKDtKas</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/HDfRMTO9p0c</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/KPOq3lP-VFg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/8808fwHl8jE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/C0KlqWbYGwI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/kHgldOcCdY8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/OGfC1tmf838</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/Jmm5hwEqnAM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/JfqeVBe7c1o</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/YK0f6ZmKEOM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/6VvfvfCj88A</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/DJEPi-yqtxI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/aM1iSdpTbfA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/2rimEkw0lc8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/ErvFlEYNWmQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/m2mxY2vp1u4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/ktpKlKTiGO4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/IRjMUt-jNio</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/fwffoPQVeYE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/1fRvMJoJGGI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/IOXIZmzSDx8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/zj8r454LfO4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/pNrWP3BcdTg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/rcQk8M6YGzU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/9PBG6TFJRug</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/JOCHuqvn1_g</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/c3IhnqGHt88</t>
   </si>
 </sst>
 </file>
@@ -1184,7 +1184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71224FC-8233-4372-B3AC-ED209CD2EB9B}">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated with JavaScript - string handling, variables, array, for loop
</commit_message>
<xml_diff>
--- a/media-data.xlsx
+++ b/media-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my-academy\learning-videos\fsd-part2-ng-java\fsd-part2-ng-java-draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAB7D2C-697C-4AFC-9B96-1C1C97901DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C8F2F2-2DF1-4CC8-8BB7-A53C4498FF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{B52A62E0-993B-4205-95A1-E40361DFFE6B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B52A62E0-993B-4205-95A1-E40361DFFE6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="370">
   <si>
     <t>id</t>
   </si>
@@ -813,6 +813,336 @@
   </si>
   <si>
     <t>https://www.youtube.com/embed/c3IhnqGHt88</t>
+  </si>
+  <si>
+    <t>JavaScript - Variables, String Literals and String Concatenation</t>
+  </si>
+  <si>
+    <t>1005</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>1002</t>
+  </si>
+  <si>
+    <t>1003</t>
+  </si>
+  <si>
+    <t>1004</t>
+  </si>
+  <si>
+    <t>Create file for learning Variables</t>
+  </si>
+  <si>
+    <t>Define Variable</t>
+  </si>
+  <si>
+    <t>Use defined Variable</t>
+  </si>
+  <si>
+    <t>Change variable value</t>
+  </si>
+  <si>
+    <t>String Concatenation</t>
+  </si>
+  <si>
+    <t>Create file for menu names display</t>
+  </si>
+  <si>
+    <t>The 'let' variable should be unique</t>
+  </si>
+  <si>
+    <t>Define unique variables</t>
+  </si>
+  <si>
+    <t>Concatenate with div tags</t>
+  </si>
+  <si>
+    <t>Concatenate with div tags in new variable</t>
+  </si>
+  <si>
+    <t>Concatenation explained</t>
+  </si>
+  <si>
+    <t>Include third menu item</t>
+  </si>
+  <si>
+    <t>1107</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>1102</t>
+  </si>
+  <si>
+    <t>1103</t>
+  </si>
+  <si>
+    <t>1104</t>
+  </si>
+  <si>
+    <t>1105</t>
+  </si>
+  <si>
+    <t>1106</t>
+  </si>
+  <si>
+    <t>Create file for Template Literal</t>
+  </si>
+  <si>
+    <t>Block comment concatenation code</t>
+  </si>
+  <si>
+    <t>Define empty string with backtick</t>
+  </si>
+  <si>
+    <t>Include template placeholders</t>
+  </si>
+  <si>
+    <t>Update menu names page with template literals</t>
+  </si>
+  <si>
+    <t>1201</t>
+  </si>
+  <si>
+    <t>1202</t>
+  </si>
+  <si>
+    <t>1203</t>
+  </si>
+  <si>
+    <t>1204</t>
+  </si>
+  <si>
+    <t>1205</t>
+  </si>
+  <si>
+    <t>Create file for array demo</t>
+  </si>
+  <si>
+    <t>Declare array of numbers</t>
+  </si>
+  <si>
+    <t>Read array item</t>
+  </si>
+  <si>
+    <t>Array length</t>
+  </si>
+  <si>
+    <t>1301</t>
+  </si>
+  <si>
+    <t>1302</t>
+  </si>
+  <si>
+    <t>1303</t>
+  </si>
+  <si>
+    <t>1304</t>
+  </si>
+  <si>
+    <t>1401</t>
+  </si>
+  <si>
+    <t>Create file to learn 'for' loop</t>
+  </si>
+  <si>
+    <t>Print numbers from 1 to 5 using for loop</t>
+  </si>
+  <si>
+    <t>The 'for' loop construct</t>
+  </si>
+  <si>
+    <t>Initialization section of 'for' loop</t>
+  </si>
+  <si>
+    <t>End statement of 'for' loop</t>
+  </si>
+  <si>
+    <t>End condition of 'for' loop</t>
+  </si>
+  <si>
+    <t>Code execution flow of 'for' loop</t>
+  </si>
+  <si>
+    <t>Print array index numbers</t>
+  </si>
+  <si>
+    <t>Implement 'for .. of' loop</t>
+  </si>
+  <si>
+    <t>Display menu names using array and for</t>
+  </si>
+  <si>
+    <t>Implement menu names as array declaration</t>
+  </si>
+  <si>
+    <t>Implement menu names using 'for of' and Template Literals</t>
+  </si>
+  <si>
+    <t>1402</t>
+  </si>
+  <si>
+    <t>1403</t>
+  </si>
+  <si>
+    <t>1404</t>
+  </si>
+  <si>
+    <t>1405</t>
+  </si>
+  <si>
+    <t>1406</t>
+  </si>
+  <si>
+    <t>1407</t>
+  </si>
+  <si>
+    <t>1408</t>
+  </si>
+  <si>
+    <t>1409</t>
+  </si>
+  <si>
+    <t>1410</t>
+  </si>
+  <si>
+    <t>1411</t>
+  </si>
+  <si>
+    <t>1412</t>
+  </si>
+  <si>
+    <t>Print array items using 'for' loop</t>
+  </si>
+  <si>
+    <t>1413</t>
+  </si>
+  <si>
+    <t>JavaScript - DOM and String Concatenation</t>
+  </si>
+  <si>
+    <t>JavaScript - Template Literal</t>
+  </si>
+  <si>
+    <t>JavaScript - 'for' loop</t>
+  </si>
+  <si>
+    <t>JavaScript - Array</t>
+  </si>
+  <si>
+    <t>1206</t>
+  </si>
+  <si>
+    <t>Define div tags within backtick</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/g9UWXxRRgnI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/o8EzyBoy3ZU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/pebkQDQ9MjQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/kswH7btOgKs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/e4a-cMZGjGo</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/DskDYjNAOQU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/HyQwkexwnE0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/aH8f-LsZKjM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/5OwqMcYdjxM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/bh65GkT3amI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/fcmjbaHd1uY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/ksIvGO5oMfg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/-aQNxKojEe0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/BVCQ8Of62bc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/7aU8RTFSPAI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/rS-zMUVd2yU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/cX-drhxpaBM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/nWXIGU-SndA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/c0B2_R4AS4U</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/4jk-sftdJIs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/rjBpMQDmi8c</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/CqtWdqg72OM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/Xbkg9vjcSQw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/C5ksx7ngvno</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/WoKxUbqSoUg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/jaZpnAh07oc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/5wgut5SP2aw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/A0oubuO9_ZY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/RrUJNeV7cR0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/FldJzVXVRgE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/ZPqjUuDu1pA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/vZ4DDzDE8LQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/UZfLeKz9Fhk</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/-SBDuMCu55s</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/rZGpuaDw5WQ</t>
   </si>
 </sst>
 </file>
@@ -1182,10 +1512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71224FC-8233-4372-B3AC-ED209CD2EB9B}">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2624,6 +2954,601 @@
         <v>259</v>
       </c>
     </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>260</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D85" t="s">
+        <v>266</v>
+      </c>
+      <c r="E85" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>260</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D86" t="s">
+        <v>267</v>
+      </c>
+      <c r="E86" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>260</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D87" t="s">
+        <v>268</v>
+      </c>
+      <c r="E87" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>260</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D88" t="s">
+        <v>269</v>
+      </c>
+      <c r="E88" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>260</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D89" t="s">
+        <v>270</v>
+      </c>
+      <c r="E89" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>329</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D90" t="s">
+        <v>271</v>
+      </c>
+      <c r="E90" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>329</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D91" t="s">
+        <v>272</v>
+      </c>
+      <c r="E91" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>329</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D92" t="s">
+        <v>273</v>
+      </c>
+      <c r="E92" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>329</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D93" t="s">
+        <v>274</v>
+      </c>
+      <c r="E93" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>329</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D94" t="s">
+        <v>275</v>
+      </c>
+      <c r="E94" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>329</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D95" t="s">
+        <v>276</v>
+      </c>
+      <c r="E95" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>329</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D96" t="s">
+        <v>277</v>
+      </c>
+      <c r="E96" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>330</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D97" t="s">
+        <v>285</v>
+      </c>
+      <c r="E97" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>330</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D98" t="s">
+        <v>286</v>
+      </c>
+      <c r="E98" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>330</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D99" t="s">
+        <v>287</v>
+      </c>
+      <c r="E99" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>330</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D100" t="s">
+        <v>334</v>
+      </c>
+      <c r="E100" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>330</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D101" t="s">
+        <v>288</v>
+      </c>
+      <c r="E101" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>330</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D102" t="s">
+        <v>289</v>
+      </c>
+      <c r="E102" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>332</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D103" t="s">
+        <v>295</v>
+      </c>
+      <c r="E103" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>332</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D104" t="s">
+        <v>296</v>
+      </c>
+      <c r="E104" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>332</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D105" t="s">
+        <v>297</v>
+      </c>
+      <c r="E105" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>332</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D106" t="s">
+        <v>298</v>
+      </c>
+      <c r="E106" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>331</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D107" t="s">
+        <v>304</v>
+      </c>
+      <c r="E107" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>331</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D108" t="s">
+        <v>305</v>
+      </c>
+      <c r="E108" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>331</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E109" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>331</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D110" t="s">
+        <v>307</v>
+      </c>
+      <c r="E110" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>331</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D111" t="s">
+        <v>308</v>
+      </c>
+      <c r="E111" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>331</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D112" t="s">
+        <v>309</v>
+      </c>
+      <c r="E112" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>331</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D113" t="s">
+        <v>310</v>
+      </c>
+      <c r="E113" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>331</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D114" t="s">
+        <v>311</v>
+      </c>
+      <c r="E114" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>331</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D115" t="s">
+        <v>327</v>
+      </c>
+      <c r="E115" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>331</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D116" t="s">
+        <v>312</v>
+      </c>
+      <c r="E116" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>331</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D117" t="s">
+        <v>313</v>
+      </c>
+      <c r="E117" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>331</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D118" t="s">
+        <v>314</v>
+      </c>
+      <c r="E118" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>331</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D119" t="s">
+        <v>315</v>
+      </c>
+      <c r="E119" t="s">
+        <v>369</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
included the operators, object, external script
</commit_message>
<xml_diff>
--- a/media-data.xlsx
+++ b/media-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my-academy\learning-videos\fsd-part2-ng-java\fsd-part2-ng-java-draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C8F2F2-2DF1-4CC8-8BB7-A53C4498FF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A633406-9414-4174-87B0-2B507AFBB6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B52A62E0-993B-4205-95A1-E40361DFFE6B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{B52A62E0-993B-4205-95A1-E40361DFFE6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="421">
   <si>
     <t>id</t>
   </si>
@@ -1143,6 +1143,159 @@
   </si>
   <si>
     <t>https://www.youtube.com/embed/rZGpuaDw5WQ</t>
+  </si>
+  <si>
+    <t>JavaScript - Operators</t>
+  </si>
+  <si>
+    <t>1501</t>
+  </si>
+  <si>
+    <t>Assignment Operator</t>
+  </si>
+  <si>
+    <t>Arithmetic Operator</t>
+  </si>
+  <si>
+    <t>Comparison Operator</t>
+  </si>
+  <si>
+    <t>1502</t>
+  </si>
+  <si>
+    <t>1503</t>
+  </si>
+  <si>
+    <t>JavaScript - Object</t>
+  </si>
+  <si>
+    <t>1601</t>
+  </si>
+  <si>
+    <t>Limitations of Variables and Arrays</t>
+  </si>
+  <si>
+    <t>Display all menu item details in console</t>
+  </si>
+  <si>
+    <t>Implement Object Array</t>
+  </si>
+  <si>
+    <t>Implement Object</t>
+  </si>
+  <si>
+    <t>Menu Object Array Walkthrough</t>
+  </si>
+  <si>
+    <t>Include Menu Object Array</t>
+  </si>
+  <si>
+    <t>Display menu based on object array</t>
+  </si>
+  <si>
+    <t>1602</t>
+  </si>
+  <si>
+    <t>1603</t>
+  </si>
+  <si>
+    <t>1604</t>
+  </si>
+  <si>
+    <t>1605</t>
+  </si>
+  <si>
+    <t>1606</t>
+  </si>
+  <si>
+    <t>1607</t>
+  </si>
+  <si>
+    <t>JavaScript - External Script</t>
+  </si>
+  <si>
+    <t>1701</t>
+  </si>
+  <si>
+    <t>External JavaScript</t>
+  </si>
+  <si>
+    <t>Copy menu object array script file</t>
+  </si>
+  <si>
+    <t>Create HTML for learning external script</t>
+  </si>
+  <si>
+    <t>Remove array declaration</t>
+  </si>
+  <si>
+    <t>Include script tag</t>
+  </si>
+  <si>
+    <t>Script tags code execution flow</t>
+  </si>
+  <si>
+    <t>1702</t>
+  </si>
+  <si>
+    <t>1703</t>
+  </si>
+  <si>
+    <t>1704</t>
+  </si>
+  <si>
+    <t>1705</t>
+  </si>
+  <si>
+    <t>1706</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/fcRHTqo9WvU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/JqtHkK0Tc8c</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/YRkleNBoGi0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/CjGEW-y_F5k</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/-HRBaPd9l5Q</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/VtMOkEAN5II</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/oZ_TcTAUDco</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/QIMZ8TrEIXg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/FOMuVv3mWXs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/e79er5dw_Eo</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/zNfz68dFlRE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/CiYlUmaTsjs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/i-hUchsNmCw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/VM9yyE3_WT0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/JtMkzEh4q6E</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/ZLW4FxYBX28</t>
   </si>
 </sst>
 </file>
@@ -1512,10 +1665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71224FC-8233-4372-B3AC-ED209CD2EB9B}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3549,6 +3702,278 @@
         <v>369</v>
       </c>
     </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>370</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D120" t="s">
+        <v>372</v>
+      </c>
+      <c r="E120" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>370</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="D121" t="s">
+        <v>373</v>
+      </c>
+      <c r="E121" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>370</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="D122" t="s">
+        <v>374</v>
+      </c>
+      <c r="E122" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>377</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D123" t="s">
+        <v>379</v>
+      </c>
+      <c r="E123" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>377</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D124" t="s">
+        <v>380</v>
+      </c>
+      <c r="E124" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>377</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="D125" t="s">
+        <v>382</v>
+      </c>
+      <c r="E125" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>377</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D126" t="s">
+        <v>381</v>
+      </c>
+      <c r="E126" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>377</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D127" t="s">
+        <v>383</v>
+      </c>
+      <c r="E127" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>377</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D128" t="s">
+        <v>384</v>
+      </c>
+      <c r="E128" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>377</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D129" t="s">
+        <v>385</v>
+      </c>
+      <c r="E129" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>392</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D130" t="s">
+        <v>394</v>
+      </c>
+      <c r="E130" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>392</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D131" t="s">
+        <v>395</v>
+      </c>
+      <c r="E131" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
+        <v>392</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D132" t="s">
+        <v>396</v>
+      </c>
+      <c r="E132" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133" t="s">
+        <v>392</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="D133" t="s">
+        <v>397</v>
+      </c>
+      <c r="E133" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134" t="s">
+        <v>392</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D134" t="s">
+        <v>398</v>
+      </c>
+      <c r="E134" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135" t="s">
+        <v>392</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D135" t="s">
+        <v>399</v>
+      </c>
+      <c r="E135" t="s">
+        <v>420</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
include till display of menu items using javascript
</commit_message>
<xml_diff>
--- a/media-data.xlsx
+++ b/media-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my-academy\learning-videos\fsd-part2-ng-java\fsd-part2-ng-java-draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A633406-9414-4174-87B0-2B507AFBB6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5FABE1-921C-4664-9BBE-13DA6AB2A642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{B52A62E0-993B-4205-95A1-E40361DFFE6B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{B52A62E0-993B-4205-95A1-E40361DFFE6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="529">
   <si>
     <t>id</t>
   </si>
@@ -1296,6 +1296,330 @@
   </si>
   <si>
     <t>https://www.youtube.com/embed/ZLW4FxYBX28</t>
+  </si>
+  <si>
+    <t>1801</t>
+  </si>
+  <si>
+    <t>Create html file for module</t>
+  </si>
+  <si>
+    <t>1802</t>
+  </si>
+  <si>
+    <t>Export menu object array</t>
+  </si>
+  <si>
+    <t>Comment external script in html</t>
+  </si>
+  <si>
+    <t>Convert script to module</t>
+  </si>
+  <si>
+    <t>Import to use menu object array</t>
+  </si>
+  <si>
+    <t>Advantages of modules explained</t>
+  </si>
+  <si>
+    <t>1901</t>
+  </si>
+  <si>
+    <t>Create html for 'if' statement demo</t>
+  </si>
+  <si>
+    <t>Include 'if' statement</t>
+  </si>
+  <si>
+    <t>Conditional 'if' statement explained</t>
+  </si>
+  <si>
+    <t>Code indentation rules</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>Significance of functions</t>
+  </si>
+  <si>
+    <t>Definition of function</t>
+  </si>
+  <si>
+    <t>Calling the function</t>
+  </si>
+  <si>
+    <t>Function and code execution flow</t>
+  </si>
+  <si>
+    <t>Passing values to a function</t>
+  </si>
+  <si>
+    <t>Return value from a function</t>
+  </si>
+  <si>
+    <t>2101</t>
+  </si>
+  <si>
+    <t>Displaying all menu items</t>
+  </si>
+  <si>
+    <t>Select all image files</t>
+  </si>
+  <si>
+    <t>Exclude first menu item in selection and copy</t>
+  </si>
+  <si>
+    <t>Create script for menu page and include import</t>
+  </si>
+  <si>
+    <t>Logic to display menu items</t>
+  </si>
+  <si>
+    <t>Menu page html code formatting</t>
+  </si>
+  <si>
+    <t>Collapse menu item div tag and copy</t>
+  </si>
+  <si>
+    <t>Define div tag template literal in menu script</t>
+  </si>
+  <si>
+    <t>Include template literal placeholders</t>
+  </si>
+  <si>
+    <t>Include properties in placeholders</t>
+  </si>
+  <si>
+    <t>Include 'id' for row div</t>
+  </si>
+  <si>
+    <t>Comment row div content</t>
+  </si>
+  <si>
+    <t>Include menu script in menu page</t>
+  </si>
+  <si>
+    <t>Display menu details using DOM</t>
+  </si>
+  <si>
+    <t>Display only active items using 'if' condition</t>
+  </si>
+  <si>
+    <t>Function to convert menu object to html</t>
+  </si>
+  <si>
+    <t>Advantage of function of menu div conversion</t>
+  </si>
+  <si>
+    <t>Bottom margin for menu items</t>
+  </si>
+  <si>
+    <t>JavaScript - Module</t>
+  </si>
+  <si>
+    <t>JavaScript - Function</t>
+  </si>
+  <si>
+    <t>JavaScript - 'if' statement</t>
+  </si>
+  <si>
+    <t>Patisserie - Display menu items using JavaScript menu objects</t>
+  </si>
+  <si>
+    <t>1803</t>
+  </si>
+  <si>
+    <t>1804</t>
+  </si>
+  <si>
+    <t>1805</t>
+  </si>
+  <si>
+    <t>1806</t>
+  </si>
+  <si>
+    <t>1902</t>
+  </si>
+  <si>
+    <t>1903</t>
+  </si>
+  <si>
+    <t>1904</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2102</t>
+  </si>
+  <si>
+    <t>2103</t>
+  </si>
+  <si>
+    <t>2104</t>
+  </si>
+  <si>
+    <t>2105</t>
+  </si>
+  <si>
+    <t>2106</t>
+  </si>
+  <si>
+    <t>2107</t>
+  </si>
+  <si>
+    <t>2108</t>
+  </si>
+  <si>
+    <t>2109</t>
+  </si>
+  <si>
+    <t>2110</t>
+  </si>
+  <si>
+    <t>2111</t>
+  </si>
+  <si>
+    <t>2112</t>
+  </si>
+  <si>
+    <t>2113</t>
+  </si>
+  <si>
+    <t>2114</t>
+  </si>
+  <si>
+    <t>2115</t>
+  </si>
+  <si>
+    <t>2116</t>
+  </si>
+  <si>
+    <t>2117</t>
+  </si>
+  <si>
+    <t>2118</t>
+  </si>
+  <si>
+    <t>2119</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/AjGgauhpK_M</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/68ZUeNVGu0k</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/rmn03WMdiaU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/5d_w0JU_FQs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/aqO6mycyoLo</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/oRxvduGkg7E</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/02hU3q0xOOg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/SaQ3tYC1hWU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/KHzocx4_jSg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/R1C6ytRg9iY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/u0crhZSNhDo</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/t8w6FQWcNac</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/5KKgepsCUyA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/znnr8G_vwKU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/AVVV1uG3Fn0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/VB_rokYGjlk</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/Bw2Zk-Yh7yI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/GRxP4AxlcNA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/5NQLwYxAlhk</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/XaItWNkMLb0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/D1rAdOAlCJU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/u4OUHLA3u-o</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/31N22kvRjA4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/Ga2eNCsjQMw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/E58jNx7m5qc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/rby7LqIAw-4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/OxdZrX6Yg4U</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/1hf3mYLWdXY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/3y_DzfrdgEc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/h2kZVL9nQh8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/hwKMQsYvh6c</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/giQG9dQtJtw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/eIu46oT_TgI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/EYhdc7T6BSY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/q5ce1nwokCk</t>
   </si>
 </sst>
 </file>
@@ -1346,10 +1670,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1665,10 +1990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71224FC-8233-4372-B3AC-ED209CD2EB9B}">
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="E137" sqref="E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3974,6 +4299,601 @@
         <v>420</v>
       </c>
     </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136" t="s">
+        <v>460</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D136" t="s">
+        <v>422</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137" t="s">
+        <v>460</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="D137" t="s">
+        <v>424</v>
+      </c>
+      <c r="E137" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138" t="s">
+        <v>460</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="D138" t="s">
+        <v>425</v>
+      </c>
+      <c r="E138" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139" t="s">
+        <v>460</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="D139" t="s">
+        <v>426</v>
+      </c>
+      <c r="E139" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140" t="s">
+        <v>460</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="D140" t="s">
+        <v>427</v>
+      </c>
+      <c r="E140" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>460</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="D141" t="s">
+        <v>428</v>
+      </c>
+      <c r="E141" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142" t="s">
+        <v>462</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D142" t="s">
+        <v>430</v>
+      </c>
+      <c r="E142" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143" t="s">
+        <v>462</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="D143" t="s">
+        <v>431</v>
+      </c>
+      <c r="E143" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144" t="s">
+        <v>462</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E144" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145" t="s">
+        <v>462</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="D145" t="s">
+        <v>433</v>
+      </c>
+      <c r="E145" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
+        <v>461</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D146" t="s">
+        <v>435</v>
+      </c>
+      <c r="E146" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147" t="s">
+        <v>461</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="D147" t="s">
+        <v>436</v>
+      </c>
+      <c r="E147" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148" t="s">
+        <v>461</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="D148" t="s">
+        <v>437</v>
+      </c>
+      <c r="E148" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149" t="s">
+        <v>461</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="D149" t="s">
+        <v>438</v>
+      </c>
+      <c r="E149" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150" t="s">
+        <v>461</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="D150" t="s">
+        <v>439</v>
+      </c>
+      <c r="E150" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>461</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D151" t="s">
+        <v>440</v>
+      </c>
+      <c r="E151" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152" t="s">
+        <v>463</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="D152" t="s">
+        <v>442</v>
+      </c>
+      <c r="E152" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153" t="s">
+        <v>463</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="D153" t="s">
+        <v>443</v>
+      </c>
+      <c r="E153" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154" t="s">
+        <v>463</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="D154" t="s">
+        <v>444</v>
+      </c>
+      <c r="E154" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155" t="s">
+        <v>463</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="D155" t="s">
+        <v>395</v>
+      </c>
+      <c r="E155" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156" t="s">
+        <v>463</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="D156" t="s">
+        <v>445</v>
+      </c>
+      <c r="E156" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157" t="s">
+        <v>463</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="D157" t="s">
+        <v>446</v>
+      </c>
+      <c r="E157" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158" t="s">
+        <v>463</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="D158" t="s">
+        <v>447</v>
+      </c>
+      <c r="E158" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159" t="s">
+        <v>463</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="D159" t="s">
+        <v>448</v>
+      </c>
+      <c r="E159" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160" t="s">
+        <v>463</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="D160" t="s">
+        <v>449</v>
+      </c>
+      <c r="E160" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161" t="s">
+        <v>463</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="D161" t="s">
+        <v>450</v>
+      </c>
+      <c r="E161" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162" t="s">
+        <v>463</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="D162" t="s">
+        <v>451</v>
+      </c>
+      <c r="E162" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163" t="s">
+        <v>463</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="D163" t="s">
+        <v>452</v>
+      </c>
+      <c r="E163" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164" t="s">
+        <v>463</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="D164" t="s">
+        <v>453</v>
+      </c>
+      <c r="E164" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165" t="s">
+        <v>463</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="D165" t="s">
+        <v>454</v>
+      </c>
+      <c r="E165" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166" t="s">
+        <v>463</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="D166" t="s">
+        <v>455</v>
+      </c>
+      <c r="E166" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167" t="s">
+        <v>463</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="D167" t="s">
+        <v>456</v>
+      </c>
+      <c r="E167" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168" t="s">
+        <v>463</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="D168" t="s">
+        <v>457</v>
+      </c>
+      <c r="E168" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169" t="s">
+        <v>463</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="D169" t="s">
+        <v>458</v>
+      </c>
+      <c r="E169" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" t="s">
+        <v>463</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="D170" t="s">
+        <v>459</v>
+      </c>
+      <c r="E170" t="s">
+        <v>528</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>